<commit_message>
docs: update README.md with correct setup and usage instructions
</commit_message>
<xml_diff>
--- a/src/main/resources/03 Form Listesi.xlsx
+++ b/src/main/resources/03 Form Listesi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmetoflu\Desktop\ahmtrdm\material\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmetoflu\Desktop\ahmtrdm\material\Archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61BF85F-5FC6-4098-9AE2-7F611A1F93C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515EF66D-AAF9-431D-83D0-39CFB41CA199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{0D52DB73-6D49-4C18-8B3C-CA2A4EF74F3F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="131">
   <si>
     <t>NO</t>
   </si>
@@ -406,12 +406,6 @@
     <t>F26</t>
   </si>
   <si>
-    <t>Topografya</t>
-  </si>
-  <si>
-    <t>Deniz Organizma</t>
-  </si>
-  <si>
     <t>Paralel Ekstrüzyon
 Doğrusal</t>
   </si>
@@ -453,6 +447,9 @@
   </si>
   <si>
     <t>Yüksek cins topoloji</t>
+  </si>
+  <si>
+    <t>Deniz Organizmaları</t>
   </si>
 </sst>
 </file>
@@ -879,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD43BDA2-CC13-44A0-8D90-BCFC18A32DB0}">
   <dimension ref="B1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -933,10 +930,10 @@
         <v>93</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E3" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" ref="E3:E28" si="0">ROW()-ROW($E$2)</f>
         <v>1</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -954,10 +951,10 @@
         <v>94</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E4" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -975,10 +972,10 @@
         <v>95</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E5" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -996,10 +993,10 @@
         <v>96</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E6" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -1017,10 +1014,10 @@
         <v>97</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E7" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F7" s="4" t="s">
@@ -1038,10 +1035,10 @@
         <v>98</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E8" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -1059,10 +1056,10 @@
         <v>99</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E9" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F9" s="4" t="s">
@@ -1080,10 +1077,10 @@
         <v>100</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E10" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F10" s="4" t="s">
@@ -1101,10 +1098,10 @@
         <v>101</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E11" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="F11" s="4" t="s">
@@ -1122,10 +1119,10 @@
         <v>102</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E12" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F12" s="4" t="s">
@@ -1143,10 +1140,10 @@
         <v>103</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E13" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F13" s="4" t="s">
@@ -1170,7 +1167,7 @@
         <v>29</v>
       </c>
       <c r="E14" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F14" s="4" t="s">
@@ -1192,7 +1189,7 @@
         <v>63</v>
       </c>
       <c r="E15" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="F15" s="4" t="s">
@@ -1214,7 +1211,7 @@
         <v>67</v>
       </c>
       <c r="E16" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="F16" s="4" t="s">
@@ -1236,7 +1233,7 @@
         <v>32</v>
       </c>
       <c r="E17" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="F17" s="4" t="s">
@@ -1258,7 +1255,7 @@
         <v>44</v>
       </c>
       <c r="E18" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="F18" s="4" t="s">
@@ -1277,10 +1274,10 @@
         <v>109</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>119</v>
+        <v>44</v>
       </c>
       <c r="E19" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="F19" s="4" t="s">
@@ -1302,7 +1299,7 @@
         <v>46</v>
       </c>
       <c r="E20" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="F20" s="4" t="s">
@@ -1326,7 +1323,7 @@
         <v>34</v>
       </c>
       <c r="E21" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="F21" s="4" t="s">
@@ -1347,7 +1344,7 @@
         <v>48</v>
       </c>
       <c r="E22" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F22" s="4" t="s">
@@ -1368,7 +1365,7 @@
         <v>37</v>
       </c>
       <c r="E23" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="F23" s="4" t="s">
@@ -1392,7 +1389,7 @@
         <v>41</v>
       </c>
       <c r="E24" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="F24" s="4" t="s">
@@ -1414,7 +1411,7 @@
         <v>51</v>
       </c>
       <c r="E25" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="F25" s="4" t="s">
@@ -1433,10 +1430,10 @@
         <v>116</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E26" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="F26" s="4" t="s">
@@ -1458,7 +1455,7 @@
         <v>81</v>
       </c>
       <c r="E27" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="F27" s="4" t="s">
@@ -1480,7 +1477,7 @@
         <v>82</v>
       </c>
       <c r="E28" s="2">
-        <f>ROW()-ROW($E$2)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="F28" s="4" t="s">

</xml_diff>